<commit_message>
Adding tabs is fixed
</commit_message>
<xml_diff>
--- a/Files/Groepskas 2324.xlsx
+++ b/Files/Groepskas 2324.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\ScoutsWallet\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36168CAE-EDA4-4E5D-8189-BD78EAEB1D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA7F352-C80F-4CB5-9606-148AC3CC2C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemeen" sheetId="1" r:id="rId1"/>
@@ -19,25 +19,12 @@
     <sheet name="Groepsreis" sheetId="4" r:id="rId4"/>
     <sheet name="Sjabloon" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="178">
   <si>
     <t>Beschrijving</t>
   </si>
@@ -4575,7 +4562,7 @@
       </c>
       <c r="E3" s="2">
         <f>SUM((B:B))</f>
-        <v>110.75</v>
+        <v>126.75</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4991,7 +4978,12 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="13">
+        <v>16</v>
+      </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>

</xml_diff>

<commit_message>
Abreviation recognition and threading
</commit_message>
<xml_diff>
--- a/Files/Groepskas 2324.xlsx
+++ b/Files/Groepskas 2324.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\ScoutsWallet\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA7F352-C80F-4CB5-9606-148AC3CC2C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701DD0B8-9FBD-4512-AA11-213AAB08171B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemeen" sheetId="1" r:id="rId1"/>

</xml_diff>